<commit_message>
Update CIERRE DE PAGOS DICIEMBRE 2025.xlsx
</commit_message>
<xml_diff>
--- a/CIERRE DE PAGOS DICIEMBRE 2025.xlsx
+++ b/CIERRE DE PAGOS DICIEMBRE 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\REPORTE MENSUAL WORLDTEL\DASHBOARD COMPARATIVO INTERNO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\REPORTE MENSUAL WORLDTEL\DASHBOARD COMPARATIVO INTERNO\COMPARATIVA-CIERRE-PAGOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E20143F7-C9D1-4302-8744-F2B2208C50D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E714F4E-8D97-4851-9178-3E2FD6E0FBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cierre_pagos_202512_ (18)" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="111">
   <si>
     <t>ID_OBLIGACION</t>
   </si>
@@ -90,9 +90,6 @@
     <t>PRIMA_AFP_PRESUNTA</t>
   </si>
   <si>
-    <t>SIN PAGO</t>
-  </si>
-  <si>
     <t>SANDRA BENAVIDES</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>CARRANZA CHILMAZA JORGE LUIS</t>
   </si>
   <si>
-    <t>F001-00035520</t>
-  </si>
-  <si>
     <t>DEUDA REAL TOTAL</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>encargado de pago</t>
   </si>
   <si>
-    <t>F001-00035571</t>
-  </si>
-  <si>
     <t>BUSY BIZ SOLUTIONS S.A.C.</t>
   </si>
   <si>
@@ -165,24 +156,12 @@
     <t>NARVAEZ YSELA MIRIAM</t>
   </si>
   <si>
-    <t>F001-00035572</t>
-  </si>
-  <si>
     <t>HINOSTROZA GOMEZ JOSE</t>
   </si>
   <si>
     <t>RABANAL MISARI ANA MARIA</t>
   </si>
   <si>
-    <t>F001-00035568</t>
-  </si>
-  <si>
-    <t>REPRESENTACIONES E &amp; N PALOMINO S.A.C.</t>
-  </si>
-  <si>
-    <t>ARIANA</t>
-  </si>
-  <si>
     <t>BONILLA PEREZ JHON ARMANDO</t>
   </si>
   <si>
@@ -229,12 +208,165 @@
   </si>
   <si>
     <t>SERVICIOS MOBILES INTERNACIONALES SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>F001-00035516</t>
+  </si>
+  <si>
+    <t>F001-00035640</t>
+  </si>
+  <si>
+    <t>F001-00035561</t>
+  </si>
+  <si>
+    <t>F001-00035567</t>
+  </si>
+  <si>
+    <t>F001-00035563</t>
+  </si>
+  <si>
+    <t>PARCIAL</t>
+  </si>
+  <si>
+    <t>201401|201402|201403|201405|201406|201407|201408|201409|201411|201412|201501|201502|201503|201505</t>
+  </si>
+  <si>
+    <t>201101|201102|201103|201105|201106|201107|201108|201109|201111|201112|201301|201302|201303|201305|201306|201307|201308|201309|201311|201312</t>
+  </si>
+  <si>
+    <t>F001-00035653</t>
+  </si>
+  <si>
+    <t>F001-00035655</t>
+  </si>
+  <si>
+    <t>F001-00035656</t>
+  </si>
+  <si>
+    <t>F001-00035661</t>
+  </si>
+  <si>
+    <t>F001-00035676</t>
+  </si>
+  <si>
+    <t>F001-00035677</t>
+  </si>
+  <si>
+    <t>F001-00035681</t>
+  </si>
+  <si>
+    <t>200709|200711|200712|200801|200802|200803|200805|200806|200807|200808|200809|200811|200812|200901|200902|200903|200905|200906|200907|200908|200909|200</t>
+  </si>
+  <si>
+    <t>201107|201109|201110|201111|201112|201201|201203|201204|201205|201206|201208|201210</t>
+  </si>
+  <si>
+    <t>F001-00035685</t>
+  </si>
+  <si>
+    <t>GRUPO SAIM E.I.R.L</t>
+  </si>
+  <si>
+    <t>RUTH</t>
+  </si>
+  <si>
+    <t>P &amp; J DISTRIBUIDORA S.A.C.</t>
+  </si>
+  <si>
+    <t>ALDAIR</t>
+  </si>
+  <si>
+    <t>PROVEEDORES Y SERVICIOS INDUSTRIALES PSI E.I.R.L.</t>
+  </si>
+  <si>
+    <t>OSCAR GUEVARA</t>
+  </si>
+  <si>
+    <t>REYES CANALES ALAN CARLOS</t>
+  </si>
+  <si>
+    <t>KATERIN</t>
+  </si>
+  <si>
+    <t>COSMOPOLITAN PERU S.A.C</t>
+  </si>
+  <si>
+    <t>CARLOS</t>
+  </si>
+  <si>
+    <t>TRANSPORTES YTUZA EMPRESA INDIVIDUAL DE RESPONSABILIDAD LIMITADA - TRANSPORTES YTUZA E.I.R.L.</t>
+  </si>
+  <si>
+    <t>ELECTROMECANICA JN S.A.C.</t>
+  </si>
+  <si>
+    <t>REALBUR S.R.L.</t>
+  </si>
+  <si>
+    <t>estudiocontable_campos@hotmail.com</t>
+  </si>
+  <si>
+    <t>INCUBADORA SANTA SOFIA SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>AC PROLOGISTIC DEL PERU SAC</t>
+  </si>
+  <si>
+    <t>YRMA</t>
+  </si>
+  <si>
+    <t>EFINERGY CONSULTORA DEL PERU E.I.R.L. - EFINERGY CONSULTORA E.I.R.L.</t>
+  </si>
+  <si>
+    <t>PONCE ROJAS JORDY JULER</t>
+  </si>
+  <si>
+    <t>GRUPO NEWTON PARAISO S.A.C.</t>
+  </si>
+  <si>
+    <t>KELLY</t>
+  </si>
+  <si>
+    <t>VIDALAB CORPORATION S.A.C.</t>
+  </si>
+  <si>
+    <t>VERONICA</t>
+  </si>
+  <si>
+    <t>ADG ARQUITECTURA Y CONSTRUCCION S.A.C.</t>
+  </si>
+  <si>
+    <t>JEAN PIERRE ARELLANO</t>
+  </si>
+  <si>
+    <t>GRUPO H Y S S.R.L.</t>
+  </si>
+  <si>
+    <t>HILDA VILLAVICENCIO</t>
+  </si>
+  <si>
+    <t>H TORRES CONSULTORES &amp; CONSTRUCTORES E.I.R.L.</t>
+  </si>
+  <si>
+    <t>ELECTRONICA INDUSTRIAL 2H E.I.R.L.</t>
+  </si>
+  <si>
+    <t>CONTRATO PUENTE GRANADA</t>
+  </si>
+  <si>
+    <t>SALON NOVOA ROSA JHERALIT</t>
+  </si>
+  <si>
+    <t>DISTRIBUIDORA DE PERNOS DEL NORTE SRLTDA</t>
+  </si>
+  <si>
+    <t>CARLOS PRADO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1102,11 +1234,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1178,10 +1310,10 @@
         <v>76477345</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>15</v>
@@ -1193,7 +1325,7 @@
         <v>20605050833</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="4">
         <v>20605050833</v>
@@ -1212,10 +1344,10 @@
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -1223,10 +1355,10 @@
         <v>76474794</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>15</v>
@@ -1238,7 +1370,7 @@
         <v>20505874529</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H3" s="4">
         <v>20505874529</v>
@@ -1257,7 +1389,7 @@
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>39</v>
@@ -1268,10 +1400,10 @@
         <v>76477124</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
@@ -1283,7 +1415,7 @@
         <v>20603914296</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H4" s="4">
         <v>20603914296</v>
@@ -1302,17 +1434,19 @@
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
+      <c r="O4" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>76479084</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>15</v>
@@ -1324,7 +1458,7 @@
         <v>20612463591</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H5" s="4">
         <v>20612463591</v>
@@ -1336,15 +1470,15 @@
         <v>127</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="4">
+        <v>17</v>
+      </c>
+      <c r="L5" s="3">
         <v>202510</v>
       </c>
+      <c r="M5" s="4"/>
       <c r="N5" s="3"/>
       <c r="O5" s="4" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1352,10 +1486,10 @@
         <v>76475076</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>15</v>
@@ -1367,7 +1501,7 @@
         <v>20521886871</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H6" s="4">
         <v>20521886871</v>
@@ -1386,10 +1520,10 @@
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1397,10 +1531,10 @@
         <v>76474019</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>15</v>
@@ -1412,7 +1546,7 @@
         <v>41977629</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H7" s="4">
         <v>10419776292</v>
@@ -1427,103 +1561,111 @@
         <v>17</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <v>76477631</v>
+        <v>76514180</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F8" s="4">
-        <v>20606210176</v>
+        <v>20519499780</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="H8" s="4">
-        <v>20606210176</v>
+        <v>20519499780</v>
       </c>
       <c r="I8" s="5">
         <v>46003</v>
       </c>
       <c r="J8" s="4">
-        <v>66.099999999999994</v>
+        <v>537.66</v>
       </c>
       <c r="K8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" s="4"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>76473991</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="4">
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="4">
+        <v>40721603</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="4">
+        <v>10407216038</v>
+      </c>
+      <c r="I9" s="5">
+        <v>46004</v>
+      </c>
+      <c r="J9" s="4">
+        <v>92.14</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="3">
         <v>202510</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="4">
-        <v>20519499780</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="4">
-        <v>20519499780</v>
-      </c>
-      <c r="I9" s="5">
-        <v>46003</v>
-      </c>
-      <c r="J9" s="4">
-        <v>537.66</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
+      <c r="O9" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
-        <v>76473991</v>
+        <v>76474057</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>15</v>
@@ -1532,39 +1674,41 @@
         <v>16</v>
       </c>
       <c r="F10" s="4">
-        <v>40721603</v>
+        <v>43371623</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H10" s="4">
-        <v>10407216038</v>
+        <v>10433716235</v>
       </c>
       <c r="I10" s="5">
         <v>46004</v>
       </c>
       <c r="J10" s="4">
-        <v>92.14</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="4">
-        <v>202510</v>
+      <c r="L10" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="O10" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
-        <v>76474057</v>
+        <v>76476539</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>15</v>
@@ -1573,39 +1717,43 @@
         <v>16</v>
       </c>
       <c r="F11" s="4">
-        <v>43371623</v>
+        <v>20601897823</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H11" s="4">
-        <v>10433716235</v>
+        <v>20601897823</v>
       </c>
       <c r="I11" s="5">
-        <v>46004</v>
+        <v>46005</v>
       </c>
       <c r="J11" s="4">
-        <v>66.099999999999994</v>
+        <v>156.71</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="4" t="s">
-        <v>30</v>
+      <c r="L11" s="4">
+        <v>202510</v>
       </c>
       <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
-        <v>76476539</v>
+        <v>76476023</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>15</v>
@@ -1614,19 +1762,19 @@
         <v>16</v>
       </c>
       <c r="F12" s="4">
-        <v>20601897823</v>
+        <v>20600140451</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H12" s="4">
-        <v>20601897823</v>
+        <v>20600140451</v>
       </c>
       <c r="I12" s="5">
-        <v>46005</v>
+        <v>46003</v>
       </c>
       <c r="J12" s="4">
-        <v>156.71</v>
+        <v>101.73</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>17</v>
@@ -1635,102 +1783,106 @@
         <v>202510</v>
       </c>
       <c r="M12" s="3"/>
-      <c r="N12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="N12" s="4"/>
+      <c r="O12" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
-        <v>76476023</v>
+        <v>76487964</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="F13" s="4">
-        <v>20600140451</v>
+        <v>20170417543</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H13" s="4">
-        <v>20600140451</v>
+        <v>20170417543</v>
       </c>
       <c r="I13" s="5">
-        <v>46003</v>
+        <v>46006</v>
       </c>
       <c r="J13" s="4">
-        <v>101.73</v>
+        <v>61.1</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="L13" s="4">
-        <v>202510</v>
+        <v>199807</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="O13" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
-        <v>76487964</v>
+        <v>76474266</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="F14" s="4">
-        <v>20170417543</v>
+        <v>20302061425</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H14" s="4">
-        <v>20170417543</v>
+        <v>20302061425</v>
       </c>
       <c r="I14" s="5">
         <v>46006</v>
       </c>
       <c r="J14" s="4">
-        <v>61.1</v>
+        <v>191.75</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="L14" s="4">
-        <v>199807</v>
+        <v>202510</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="O14" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
-        <v>76474266</v>
+        <v>76477210</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>15</v>
@@ -1739,19 +1891,19 @@
         <v>16</v>
       </c>
       <c r="F15" s="4">
-        <v>20302061425</v>
+        <v>20604322678</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H15" s="4">
-        <v>20302061425</v>
+        <v>20604322678</v>
       </c>
       <c r="I15" s="5">
         <v>46006</v>
       </c>
       <c r="J15" s="4">
-        <v>191.75</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>17</v>
@@ -1760,96 +1912,108 @@
         <v>202510</v>
       </c>
       <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
-        <v>76477210</v>
+        <v>76513681</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F16" s="4">
-        <v>20604322678</v>
+        <v>20509470848</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H16" s="4">
-        <v>20604322678</v>
+        <v>20509470848</v>
       </c>
       <c r="I16" s="5">
         <v>46006</v>
       </c>
       <c r="J16" s="4">
-        <v>66.099999999999994</v>
+        <v>961.77</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L16" s="4">
-        <v>202510</v>
-      </c>
-      <c r="M16" s="3"/>
-      <c r="N16" s="4" t="s">
-        <v>59</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="N16" s="4"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>76477683</v>
+      </c>
       <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F17" s="4">
-        <v>20509470848</v>
+        <v>20606399279</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H17" s="4">
-        <v>20509470848</v>
+        <v>20606399279</v>
       </c>
       <c r="I17" s="5">
         <v>46006</v>
       </c>
       <c r="J17" s="4">
-        <v>961.77</v>
-      </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+        <v>185.9</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" s="3">
+        <v>202510</v>
+      </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O17" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
-        <v>76477683</v>
+        <v>76474264</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>15</v>
@@ -1858,19 +2022,19 @@
         <v>16</v>
       </c>
       <c r="F18" s="4">
-        <v>20606399279</v>
+        <v>20298537461</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H18" s="4">
-        <v>20606399279</v>
+        <v>20298537461</v>
       </c>
       <c r="I18" s="5">
         <v>46006</v>
       </c>
       <c r="J18" s="4">
-        <v>185.9</v>
+        <v>102</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>17</v>
@@ -1879,39 +2043,41 @@
         <v>202510</v>
       </c>
       <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
+      <c r="N18" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="O18" s="3"/>
     </row>
-    <row r="19" spans="1:15" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
-        <v>76474264</v>
+        <v>76498557</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F19" s="4">
-        <v>20298537461</v>
+        <v>20514534251</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H19" s="4">
-        <v>20298537461</v>
+        <v>20514534251</v>
       </c>
       <c r="I19" s="5">
-        <v>46006</v>
+        <v>46007</v>
       </c>
       <c r="J19" s="4">
-        <v>102</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>17</v>
@@ -1920,41 +2086,39 @@
         <v>202510</v>
       </c>
       <c r="M19" s="3"/>
-      <c r="N19" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="N19" s="4"/>
       <c r="O19" s="3"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
-        <v>76498557</v>
+        <v>76474877</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F20" s="4">
-        <v>20514534251</v>
+        <v>20511763089</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H20" s="4">
-        <v>20514534251</v>
+        <v>20511763089</v>
       </c>
       <c r="I20" s="5">
         <v>46007</v>
       </c>
       <c r="J20" s="4">
-        <v>66.099999999999994</v>
+        <v>223.16</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>17</v>
@@ -1963,18 +2127,20 @@
         <v>202510</v>
       </c>
       <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="N20" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
-        <v>76474877</v>
+        <v>76478040</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>15</v>
@@ -1983,19 +2149,19 @@
         <v>16</v>
       </c>
       <c r="F21" s="4">
-        <v>20511763089</v>
+        <v>20608123696</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="H21" s="4">
-        <v>20511763089</v>
+        <v>20608123696</v>
       </c>
       <c r="I21" s="5">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="J21" s="4">
-        <v>223.16</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>17</v>
@@ -2005,9 +2171,735 @@
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="4" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>76476898</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22">
+        <v>20603066112</v>
+      </c>
+      <c r="G22" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22">
+        <v>20603066112</v>
+      </c>
+      <c r="I22">
+        <v>46008</v>
+      </c>
+      <c r="J22">
+        <v>107</v>
+      </c>
+      <c r="K22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22">
+        <v>202510</v>
+      </c>
+      <c r="N22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>76477208</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23">
+        <v>20604312583</v>
+      </c>
+      <c r="G23" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23">
+        <v>20604312583</v>
+      </c>
+      <c r="I23">
+        <v>46008</v>
+      </c>
+      <c r="J23">
+        <v>74</v>
+      </c>
+      <c r="K23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23">
+        <v>202510</v>
+      </c>
+      <c r="N23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>76474010</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24">
+        <v>41673301</v>
+      </c>
+      <c r="G24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24">
+        <v>10416733011</v>
+      </c>
+      <c r="I24">
+        <v>46008</v>
+      </c>
+      <c r="J24">
+        <v>94</v>
+      </c>
+      <c r="K24" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" t="s">
+        <v>29</v>
+      </c>
+      <c r="N24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>76475605</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25">
+        <v>20551438113</v>
+      </c>
+      <c r="G25" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25">
+        <v>20551438113</v>
+      </c>
+      <c r="I25">
+        <v>46008</v>
+      </c>
+      <c r="J25">
+        <v>139</v>
+      </c>
+      <c r="K25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" t="s">
+        <v>29</v>
+      </c>
+      <c r="N25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>76476513</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <v>20601813832</v>
+      </c>
+      <c r="G26" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26">
+        <v>20601813832</v>
+      </c>
+      <c r="I26">
+        <v>46002</v>
+      </c>
+      <c r="J26">
+        <v>123.29</v>
+      </c>
+      <c r="K26" t="s">
+        <v>17</v>
+      </c>
+      <c r="L26">
+        <v>202510</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>76475776</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27">
+        <v>20556935280</v>
+      </c>
+      <c r="G27" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27">
+        <v>20556935280</v>
+      </c>
+      <c r="I27">
+        <v>46008</v>
+      </c>
+      <c r="J27">
+        <v>131.65</v>
+      </c>
+      <c r="K27" t="s">
+        <v>17</v>
+      </c>
+      <c r="L27">
+        <v>202510</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>76476825</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>20602849636</v>
+      </c>
+      <c r="G28" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28">
+        <v>20602849636</v>
+      </c>
+      <c r="I28">
+        <v>46008</v>
+      </c>
+      <c r="J28">
+        <v>80.78</v>
+      </c>
+      <c r="K28" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" t="s">
+        <v>29</v>
+      </c>
+      <c r="N28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>76477775</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29">
+        <v>20606753820</v>
+      </c>
+      <c r="G29" t="s">
+        <v>92</v>
+      </c>
+      <c r="H29">
+        <v>20606753820</v>
+      </c>
+      <c r="I29">
+        <v>46008</v>
+      </c>
+      <c r="J29">
+        <v>71.28</v>
+      </c>
+      <c r="K29" t="s">
+        <v>17</v>
+      </c>
+      <c r="L29">
+        <v>202510</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>76474698</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30">
+        <v>20492994945</v>
+      </c>
+      <c r="G30" t="s">
+        <v>93</v>
+      </c>
+      <c r="H30">
+        <v>20492994945</v>
+      </c>
+      <c r="I30">
+        <v>46008</v>
+      </c>
+      <c r="J30">
+        <v>332</v>
+      </c>
+      <c r="K30" t="s">
+        <v>65</v>
+      </c>
+      <c r="L30">
+        <v>202510</v>
+      </c>
+      <c r="M30">
+        <v>202510</v>
+      </c>
+      <c r="N30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>76477704</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31">
+        <v>20606518235</v>
+      </c>
+      <c r="G31" t="s">
+        <v>95</v>
+      </c>
+      <c r="H31">
+        <v>20606518235</v>
+      </c>
+      <c r="I31">
+        <v>46009</v>
+      </c>
+      <c r="J31">
+        <v>71</v>
+      </c>
+      <c r="K31" t="s">
+        <v>17</v>
+      </c>
+      <c r="L31">
+        <v>202510</v>
+      </c>
+      <c r="N31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>76478655</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <v>20610621351</v>
+      </c>
+      <c r="G32" t="s">
+        <v>97</v>
+      </c>
+      <c r="H32">
+        <v>20610621351</v>
+      </c>
+      <c r="I32">
+        <v>46009</v>
+      </c>
+      <c r="J32">
+        <v>93</v>
+      </c>
+      <c r="K32" t="s">
+        <v>17</v>
+      </c>
+      <c r="L32" t="s">
+        <v>25</v>
+      </c>
+      <c r="N32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>76477598</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33">
+        <v>20606102187</v>
+      </c>
+      <c r="G33" t="s">
+        <v>99</v>
+      </c>
+      <c r="H33">
+        <v>20606102187</v>
+      </c>
+      <c r="I33">
+        <v>46008</v>
+      </c>
+      <c r="J33">
+        <v>161</v>
+      </c>
+      <c r="K33" t="s">
+        <v>17</v>
+      </c>
+      <c r="L33">
+        <v>202510</v>
+      </c>
+      <c r="N33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>76475622</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34">
+        <v>20551916970</v>
+      </c>
+      <c r="G34" t="s">
+        <v>101</v>
+      </c>
+      <c r="H34">
+        <v>20551916970</v>
+      </c>
+      <c r="I34">
+        <v>46009</v>
+      </c>
+      <c r="J34">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="K34" t="s">
+        <v>17</v>
+      </c>
+      <c r="L34">
+        <v>202510</v>
+      </c>
+      <c r="N34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>76474540</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35">
+        <v>20478157976</v>
+      </c>
+      <c r="G35" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35">
+        <v>20478157976</v>
+      </c>
+      <c r="I35">
+        <v>46009</v>
+      </c>
+      <c r="J35">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="K35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35">
+        <v>202510</v>
+      </c>
+      <c r="N35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>76475394</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36">
+        <v>20542353059</v>
+      </c>
+      <c r="G36" t="s">
+        <v>105</v>
+      </c>
+      <c r="H36">
+        <v>20542353059</v>
+      </c>
+      <c r="I36">
+        <v>46009</v>
+      </c>
+      <c r="J36">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="K36" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36">
+        <v>202510</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>76475653</v>
+      </c>
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37">
+        <v>20552638337</v>
+      </c>
+      <c r="G37" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37">
+        <v>20552638337</v>
+      </c>
+      <c r="I37">
+        <v>46009</v>
+      </c>
+      <c r="J37">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="K37" t="s">
+        <v>17</v>
+      </c>
+      <c r="L37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>76479527</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38">
+        <v>20614566842</v>
+      </c>
+      <c r="G38" t="s">
+        <v>107</v>
+      </c>
+      <c r="H38">
+        <v>20614566842</v>
+      </c>
+      <c r="I38">
+        <v>46009</v>
+      </c>
+      <c r="J38">
+        <v>132</v>
+      </c>
+      <c r="K38" t="s">
+        <v>17</v>
+      </c>
+      <c r="L38">
+        <v>202510</v>
+      </c>
+      <c r="N38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>76474203</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39">
+        <v>20113539675</v>
+      </c>
+      <c r="G39" t="s">
+        <v>109</v>
+      </c>
+      <c r="H39">
+        <v>20113539675</v>
+      </c>
+      <c r="I39">
+        <v>46010</v>
+      </c>
+      <c r="J39">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="K39" t="s">
+        <v>17</v>
+      </c>
+      <c r="L39">
+        <v>202510</v>
+      </c>
+      <c r="N39" t="s">
+        <v>110</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>